<commit_message>
Deploy v2.15.059 (2026-02-23 18:08:13)
</commit_message>
<xml_diff>
--- a/Excel & Data Files/Indoors Relays.xlsx
+++ b/Excel & Data Files/Indoors Relays.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972CD0AF-599A-6345-ABD8-A7EBE3651240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D71941D-76DB-9640-8568-01F3C4347528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="600" windowWidth="34260" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36620" yWindow="3400" windowWidth="34260" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="National Records" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Settings" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'National Records'!$A$1:$R$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'National Records'!$A$1:$R$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
   <si>
     <t>Επίδοση</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>LNAME</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -844,11 +847,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -858,8 +861,8 @@
     <col min="4" max="4" width="8.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="27" style="1" customWidth="1"/>
@@ -942,11 +945,11 @@
         <v>1</v>
       </c>
       <c r="F2" s="18" t="e">
-        <f t="shared" ref="F2:F12" si="0">LEFT(H2,FIND(" ",H2))</f>
+        <f t="shared" ref="F2:F11" si="0">LEFT(H2,FIND(" ",H2))</f>
         <v>#VALUE!</v>
       </c>
       <c r="G2" s="18" t="e">
-        <f t="shared" ref="G2:G12" si="1">MID(H2,FIND(" ",H2)+1,LEN(H2)-LEN(F2))</f>
+        <f t="shared" ref="G2:G11" si="1">MID(H2,FIND(" ",H2)+1,LEN(H2)-LEN(F2))</f>
         <v>#VALUE!</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1278,8 +1281,8 @@
       <c r="C9" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="15">
-        <v>0</v>
+      <c r="D9" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="E9" s="8">
         <v>1</v>
@@ -1295,10 +1298,31 @@
       <c r="H9" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="J9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>119</v>
@@ -1307,7 +1331,7 @@
         <v>125</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E10" s="8">
         <v>1</v>
@@ -1323,26 +1347,27 @@
       <c r="H10" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="I10" s="16"/>
       <c r="J10" s="1" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>43</v>
+        <v>74</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1356,7 +1381,7 @@
         <v>125</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E11" s="8">
         <v>1</v>
@@ -1374,75 +1399,74 @@
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E12" s="8">
         <v>1</v>
       </c>
-      <c r="F12" s="18" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G12" s="18" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="F12" s="18" t="str">
+        <f t="shared" ref="F12:F16" si="2">LEFT(H12,FIND(" ",H12))</f>
+        <v xml:space="preserve">Αγγελική </v>
+      </c>
+      <c r="G12" s="18" t="str">
+        <f t="shared" ref="G12:G16" si="3">MID(H12,FIND(" ",H12)+1,LEN(H12)-LEN(F12))</f>
+        <v>Λαμπρόγλου (8.9.1983)</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12" s="16"/>
+        <v>57</v>
+      </c>
       <c r="J12" s="1" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>81</v>
+        <v>15</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1450,48 +1474,48 @@
         <v>21</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E13" s="8">
         <v>1</v>
       </c>
       <c r="F13" s="18" t="str">
-        <f t="shared" ref="F13:F17" si="2">LEFT(H13,FIND(" ",H13))</f>
-        <v xml:space="preserve">Αγγελική </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">Άννα </v>
       </c>
       <c r="G13" s="18" t="str">
-        <f t="shared" ref="G13:G17" si="3">MID(H13,FIND(" ",H13)+1,LEN(H13)-LEN(F13))</f>
-        <v>Λαμπρόγλου (8.9.1983)</v>
+        <f t="shared" si="3"/>
+        <v>Δάφτσου (25.09.1970)</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1499,13 +1523,13 @@
         <v>21</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E14" s="8">
         <v>1</v>
@@ -1522,10 +1546,10 @@
         <v>68</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>15</v>
@@ -1537,10 +1561,10 @@
         <v>59</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1548,48 +1572,48 @@
         <v>21</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E15" s="8">
         <v>1</v>
       </c>
       <c r="F15" s="18" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">Άννα </v>
+        <v xml:space="preserve">Αθηνά </v>
       </c>
       <c r="G15" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>Δάφτσου (25.09.1970)</v>
+        <v>Βαϊνά (8.12.1959)</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1597,13 +1621,13 @@
         <v>21</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E16" s="8">
         <v>1</v>
@@ -1620,10 +1644,10 @@
         <v>49</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>15</v>
@@ -1632,66 +1656,17 @@
         <v>49</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="8">
-        <v>1</v>
-      </c>
-      <c r="F17" s="18" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">Αθηνά </v>
-      </c>
-      <c r="G17" s="18" t="str">
-        <f t="shared" si="3"/>
-        <v>Βαϊνά (8.12.1959)</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:R16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploy v2.15.054 (2026-02-23 20:16:34)
</commit_message>
<xml_diff>
--- a/Excel & Data Files/Indoors Relays.xlsx
+++ b/Excel & Data Files/Indoors Relays.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D71941D-76DB-9640-8568-01F3C4347528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972CD0AF-599A-6345-ABD8-A7EBE3651240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36620" yWindow="3400" windowWidth="34260" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7940" yWindow="600" windowWidth="34260" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="National Records" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Settings" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'National Records'!$A$1:$R$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'National Records'!$A$1:$R$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="128">
   <si>
     <t>Επίδοση</t>
   </si>
@@ -417,9 +417,6 @@
   </si>
   <si>
     <t>LNAME</t>
-  </si>
-  <si>
-    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -847,11 +844,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -861,8 +858,8 @@
     <col min="4" max="4" width="8.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="27" style="1" customWidth="1"/>
@@ -945,11 +942,11 @@
         <v>1</v>
       </c>
       <c r="F2" s="18" t="e">
-        <f t="shared" ref="F2:F11" si="0">LEFT(H2,FIND(" ",H2))</f>
+        <f t="shared" ref="F2:F12" si="0">LEFT(H2,FIND(" ",H2))</f>
         <v>#VALUE!</v>
       </c>
       <c r="G2" s="18" t="e">
-        <f t="shared" ref="G2:G11" si="1">MID(H2,FIND(" ",H2)+1,LEN(H2)-LEN(F2))</f>
+        <f t="shared" ref="G2:G12" si="1">MID(H2,FIND(" ",H2)+1,LEN(H2)-LEN(F2))</f>
         <v>#VALUE!</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1281,8 +1278,8 @@
       <c r="C9" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>95</v>
+      <c r="D9" s="15">
+        <v>0</v>
       </c>
       <c r="E9" s="8">
         <v>1</v>
@@ -1298,31 +1295,10 @@
       <c r="H9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>119</v>
@@ -1331,7 +1307,7 @@
         <v>125</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" s="8">
         <v>1</v>
@@ -1347,27 +1323,26 @@
       <c r="H10" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="16"/>
       <c r="J10" s="1" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>52</v>
+        <v>15</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1381,7 +1356,7 @@
         <v>125</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" s="8">
         <v>1</v>
@@ -1399,74 +1374,75 @@
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E12" s="8">
         <v>1</v>
       </c>
-      <c r="F12" s="18" t="str">
-        <f t="shared" ref="F12:F16" si="2">LEFT(H12,FIND(" ",H12))</f>
-        <v xml:space="preserve">Αγγελική </v>
-      </c>
-      <c r="G12" s="18" t="str">
-        <f t="shared" ref="G12:G16" si="3">MID(H12,FIND(" ",H12)+1,LEN(H12)-LEN(F12))</f>
-        <v>Λαμπρόγλου (8.9.1983)</v>
+      <c r="F12" s="18" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G12" s="18" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="I12" s="16"/>
       <c r="J12" s="1" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>57</v>
+        <v>16</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1474,48 +1450,48 @@
         <v>21</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="8">
         <v>1</v>
       </c>
       <c r="F13" s="18" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">Άννα </v>
+        <f t="shared" ref="F13:F17" si="2">LEFT(H13,FIND(" ",H13))</f>
+        <v xml:space="preserve">Αγγελική </v>
       </c>
       <c r="G13" s="18" t="str">
-        <f t="shared" si="3"/>
-        <v>Δάφτσου (25.09.1970)</v>
+        <f t="shared" ref="G13:G17" si="3">MID(H13,FIND(" ",H13)+1,LEN(H13)-LEN(F13))</f>
+        <v>Λαμπρόγλου (8.9.1983)</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1523,13 +1499,13 @@
         <v>21</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" s="8">
         <v>1</v>
@@ -1546,10 +1522,10 @@
         <v>68</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>15</v>
@@ -1561,10 +1537,10 @@
         <v>59</v>
       </c>
       <c r="P14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1572,48 +1548,48 @@
         <v>21</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" s="8">
         <v>1</v>
       </c>
       <c r="F15" s="18" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">Αθηνά </v>
+        <v xml:space="preserve">Άννα </v>
       </c>
       <c r="G15" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>Βαϊνά (8.12.1959)</v>
+        <v>Δάφτσου (25.09.1970)</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="O15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q15" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1621,13 +1597,13 @@
         <v>21</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" s="8">
         <v>1</v>
@@ -1644,10 +1620,10 @@
         <v>49</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>15</v>
@@ -1656,17 +1632,66 @@
         <v>49</v>
       </c>
       <c r="O16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">Αθηνά </v>
+      </c>
+      <c r="G17" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>Βαϊνά (8.12.1959)</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:R17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>